<commit_message>
Major correction of group allocation to solve a mixup of Thalamus and Striatal samples.
</commit_message>
<xml_diff>
--- a/input/Nextera PCR for all 25 tissues and 5 in vitro samples.xlsx
+++ b/input/Nextera PCR for all 25 tissues and 5 in vitro samples.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26621"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="840" yWindow="1360" windowWidth="25360" windowHeight="15820" tabRatio="500"/>
+    <workbookView xWindow="19700" yWindow="3660" windowWidth="25360" windowHeight="15820" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -945,8 +945,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M60"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="M34" sqref="M34"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="I33" sqref="I33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1100,7 +1100,7 @@
         <v>37</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="J4" s="2">
         <v>13.3</v>
@@ -1139,7 +1139,7 @@
         <v>37</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="J5" s="2">
         <v>9.8000000000000007</v>
@@ -1261,7 +1261,7 @@
         <v>37</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="J9" s="2">
         <v>11.06</v>
@@ -1300,7 +1300,7 @@
         <v>37</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="J10" s="2">
         <v>4.0999999999999996</v>
@@ -1419,7 +1419,7 @@
         <v>37</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="J14" s="2">
         <v>4.3</v>
@@ -1459,7 +1459,7 @@
         <v>37</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="J15" s="2">
         <v>5.26</v>
@@ -1582,7 +1582,7 @@
         <v>59</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="J19" s="2">
         <v>5.88</v>
@@ -1622,7 +1622,7 @@
         <v>59</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="J20" s="2">
         <v>4.38</v>
@@ -1745,7 +1745,7 @@
         <v>59</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="J24" s="2">
         <v>8.1999999999999993</v>
@@ -1785,7 +1785,7 @@
         <v>59</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="J25" s="2">
         <v>4.54</v>
@@ -1867,7 +1867,7 @@
         <v>59</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="J28" s="2">
         <v>9.34</v>
@@ -1906,7 +1906,7 @@
         <v>59</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="J29" s="2">
         <v>9.1</v>
@@ -1945,7 +1945,7 @@
         <v>59</v>
       </c>
       <c r="I31" s="2" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="J31" s="2">
         <v>6.04</v>
@@ -1984,7 +1984,7 @@
         <v>59</v>
       </c>
       <c r="I32" s="6" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="J32" s="6">
         <v>4.88</v>

</xml_diff>